<commit_message>
GIS foto Pekla zplozenci
</commit_message>
<xml_diff>
--- a/longitude - latitude/peklazplozenci_toponyms.xlsx
+++ b/longitude - latitude/peklazplozenci_toponyms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Změlík\Desktop\GIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Změlík\Desktop\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D2D48A-80E0-44C3-A194-8654BA6CDA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9000592-5261-4436-848B-2F1E35CEC5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1815" yWindow="15" windowWidth="23295" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>longitude</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>Novoměstská radnice</t>
+  </si>
+  <si>
+    <t>dnes Štěpánská</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -591,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,13 +614,13 @@
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -619,8 +628,11 @@
       <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -633,8 +645,14 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -647,8 +665,11 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -664,8 +685,11 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -681,8 +705,11 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -695,8 +722,11 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -709,8 +739,11 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -726,8 +759,11 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -743,8 +779,11 @@
       <c r="E9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -760,8 +799,11 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -774,8 +816,11 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -791,8 +836,11 @@
       <c r="E12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -805,8 +853,11 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -819,8 +870,11 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -833,8 +887,11 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -846,6 +903,9 @@
       </c>
       <c r="D16" t="s">
         <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>